<commit_message>
fixed iteration count in bisection method
</commit_message>
<xml_diff>
--- a/01-lab/results/golden_ratio_method_results.xlsx
+++ b/01-lab/results/golden_ratio_method_results.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="24" uniqueCount="2">
   <si>
     <t>rearranged_array_1</t>
   </si>
@@ -84,15 +84,15 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
+        <v>5</v>
+      </c>
+      <c r="B2" s="0">
         <v>2.5</v>
-      </c>
-      <c r="B2" s="0">
-        <v>7.5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>5</v>
+        <v>7.5</v>
       </c>
       <c r="B3" s="0">
         <v>2.5</v>
@@ -100,10 +100,10 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>7.5</v>
+        <v>1.25</v>
       </c>
       <c r="B4" s="0">
-        <v>2.5</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="5">
@@ -111,23 +111,23 @@
         <v>1.25</v>
       </c>
       <c r="B5" s="0">
-        <v>3.75</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
+        <v>1.875</v>
+      </c>
+      <c r="B6" s="0">
         <v>1.25</v>
-      </c>
-      <c r="B6" s="0">
-        <v>0.625</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>1.875</v>
+        <v>0.9375</v>
       </c>
       <c r="B7" s="0">
-        <v>1.25</v>
+        <v>1.5625</v>
       </c>
     </row>
     <row r="8">
@@ -135,47 +135,47 @@
         <v>0.9375</v>
       </c>
       <c r="B8" s="0">
-        <v>1.5625</v>
+        <v>0.78125</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
+        <v>1.09375</v>
+      </c>
+      <c r="B9" s="0">
         <v>0.9375</v>
-      </c>
-      <c r="B9" s="0">
-        <v>0.78125</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>1.09375</v>
+        <v>0.859375</v>
       </c>
       <c r="B10" s="0">
-        <v>0.9375</v>
+        <v>1.015625</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>0.859375</v>
+        <v>1.015625</v>
       </c>
       <c r="B11" s="0">
-        <v>1.015625</v>
+        <v>0.9765625</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
+        <v>1.0546875</v>
+      </c>
+      <c r="B12" s="0">
         <v>1.015625</v>
-      </c>
-      <c r="B12" s="0">
-        <v>0.9765625</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>1.0546875</v>
+        <v>0.99609375</v>
       </c>
       <c r="B13" s="0">
-        <v>1.015625</v>
+        <v>1.03515625</v>
       </c>
     </row>
     <row r="14">
@@ -183,47 +183,47 @@
         <v>0.99609375</v>
       </c>
       <c r="B14" s="0">
-        <v>1.03515625</v>
+        <v>0.986328125</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
+        <v>1.005859375</v>
+      </c>
+      <c r="B15" s="0">
         <v>0.99609375</v>
-      </c>
-      <c r="B15" s="0">
-        <v>0.986328125</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>1.005859375</v>
+        <v>0.9912109375</v>
       </c>
       <c r="B16" s="0">
-        <v>0.99609375</v>
+        <v>1.0009765625</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>0.9912109375</v>
+        <v>1.0009765625</v>
       </c>
       <c r="B17" s="0">
-        <v>1.0009765625</v>
+        <v>0.99853515625</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
+        <v>1.00341796875</v>
+      </c>
+      <c r="B18" s="0">
         <v>1.0009765625</v>
-      </c>
-      <c r="B18" s="0">
-        <v>0.99853515625</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>1.00341796875</v>
+        <v>0.999755859375</v>
       </c>
       <c r="B19" s="0">
-        <v>1.0009765625</v>
+        <v>1.002197265625</v>
       </c>
     </row>
     <row r="20">
@@ -231,47 +231,47 @@
         <v>0.999755859375</v>
       </c>
       <c r="B20" s="0">
-        <v>1.002197265625</v>
+        <v>0.9991455078125</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
+        <v>1.0003662109375</v>
+      </c>
+      <c r="B21" s="0">
         <v>0.999755859375</v>
-      </c>
-      <c r="B21" s="0">
-        <v>0.9991455078125</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>1.0003662109375</v>
+        <v>0.99945068359375</v>
       </c>
       <c r="B22" s="0">
-        <v>0.999755859375</v>
+        <v>1.00006103515625</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>0.99945068359375</v>
+        <v>1.00006103515625</v>
       </c>
       <c r="B23" s="0">
-        <v>1.00006103515625</v>
+        <v>0.999908447265625</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
+        <v>1.000213623046875</v>
+      </c>
+      <c r="B24" s="0">
         <v>1.00006103515625</v>
-      </c>
-      <c r="B24" s="0">
-        <v>0.999908447265625</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>1.000213623046875</v>
+        <v>0.9999847412109375</v>
       </c>
       <c r="B25" s="0">
-        <v>1.00006103515625</v>
+        <v>1.0001373291015625</v>
       </c>
     </row>
     <row r="26">
@@ -279,15 +279,15 @@
         <v>0.9999847412109375</v>
       </c>
       <c r="B26" s="0">
-        <v>1.0001373291015625</v>
+        <v>0.99994659423828125</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
+        <v>1.0000228881835938</v>
+      </c>
+      <c r="B27" s="0">
         <v>0.9999847412109375</v>
-      </c>
-      <c r="B27" s="0">
-        <v>0.99994659423828125</v>
       </c>
     </row>
     <row r="28">

</xml_diff>

<commit_message>
fixed iteration count in golden ratio method
</commit_message>
<xml_diff>
--- a/01-lab/results/golden_ratio_method_results.xlsx
+++ b/01-lab/results/golden_ratio_method_results.xlsx
@@ -13,12 +13,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="24" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="28" uniqueCount="3">
   <si>
     <t>rearranged_array_1</t>
   </si>
   <si>
     <t>rearranged_array_2</t>
+  </si>
+  <si>
+    <t>rearranged_array</t>
   </si>
 </sst>
 </file>

</xml_diff>